<commit_message>
Monitor metaG bulk submission
</commit_message>
<xml_diff>
--- a/data/docs/bulk-submissions/NMDC-EDGE-Metagenomics-pipeline-bulk-submission.xlsx
+++ b/data/docs/bulk-submissions/NMDC-EDGE-Metagenomics-pipeline-bulk-submission.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yxu/dev/node16_apps/nmdc-edge/data/docs/bulk-submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307D2FFB-40A0-6444-A33D-818C255F507E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DFE11F-03EC-2741-9182-1D0628F3EB8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="2860" windowWidth="27240" windowHeight="16440" xr2:uid="{D4B1EDC8-DFE1-D14C-9E75-173BCE7BAFAC}"/>
+    <workbookView xWindow="16620" yWindow="8200" windowWidth="27240" windowHeight="16440" xr2:uid="{D4B1EDC8-DFE1-D14C-9E75-173BCE7BAFAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$1</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -87,8 +90,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,7 +429,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{030A96EA-2FA1-8348-B17F-A091C9D7BE5F}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -453,6 +459,9 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C2" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="5">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Project/Run Name" error="Invalid Input" promptTitle="Project/Run Name" prompt="Required. At least 3 but less than 30 characters. Only alphabets, numbers, dashs, dot and underscore are allowed." sqref="A2:A100" xr:uid="{291FD160-E4F0-854B-9418-A6B8EACE1298}">
@@ -460,9 +469,9 @@
       <formula2>30</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Description" prompt="Optional" sqref="B2:B100" xr:uid="{CB3D86F2-D212-C340-9296-8EF1CAF1D742}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Pair-1 FASTQ" prompt="Your NMDC-EDGE uploaded file name(s). Separate multiple names with commas." sqref="D2:D100" xr:uid="{5FCBE9B3-9D75-384A-9086-4A4CE3DAB6D7}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Pair-2 FASTQ" prompt="Your NMDC-EDGE uploaded file name(s). Separate multiple names with commas." sqref="E2:E100" xr:uid="{9667BBE3-FF05-1C4F-A787-AC2369651A5F}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Interleaved FASTQ" prompt="Your NMDC-EDGE uploaded file name(s). Separate multiple names with commas." sqref="C2:C100" xr:uid="{776E149A-8CE7-8742-B499-CD03793E3956}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Pair-1 FASTQ" prompt="Accept uploaded files, SRA files and http(s) url inputs. Separate multiple files with commas._x000a__x000a_Examples:_x000a_upload/test_R1.fq_x000a_sra/SRR1602702.fastq.gz_x000a_https://nmdc-edge.org/publicdata/test_data/Ecoli_interleaved_pe_small.fastq" sqref="D2:D100" xr:uid="{5FCBE9B3-9D75-384A-9086-4A4CE3DAB6D7}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Pair-2 FASTQ" prompt="Accept uploaded files, SRA files and http(s) url inputs. Separate multiple files with commas._x000a__x000a_Examples:_x000a_upload/test_R1.fq_x000a_sra/SRR1602702.fastq.gz_x000a_https://nmdc-edge.org/publicdata/test_data/Ecoli_interleaved_pe_small.fastq" sqref="E2:E100" xr:uid="{9667BBE3-FF05-1C4F-A787-AC2369651A5F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Interleaved FASTQ" prompt="Accept uploaded files, SRA files and http(s) url inputs. Separate multiple files with commas._x000a__x000a_Examples:_x000a_upload/test_R1.fq_x000a_sra/SRR1602702.fastq.gz_x000a_https://nmdc-edge.org/publicdata/test_data/Ecoli_interleaved_pe_small.fastq" sqref="C2:C100" xr:uid="{776E149A-8CE7-8742-B499-CD03793E3956}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>